<commit_message>
Change Brazilian Portuguese template files on asset folder. Files created on a Brazilian Portuguese Microsoft Office 2016 install, then removed Author and saved. Previous files were either in English or Portugal Portuguese.
</commit_message>
<xml_diff>
--- a/assets/pt_BR/new.xlsx
+++ b/assets/pt_BR/new.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Tavmonster\hdd4tb\Arnosti\docs-ptbr-office2016\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,14 +24,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -70,7 +74,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -86,7 +90,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -98,7 +102,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -115,9 +119,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -145,14 +149,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -180,6 +201,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -338,5 +376,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>